<commit_message>
Data summarization using Excel and Python
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yousif Ennwa\Documents\GitHub\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D7E66D-06CA-4A14-AE4A-A5CD02F8DB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD4AEBD-9755-4312-A72B-ACF200A40753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="4" activeTab="8" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="4" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Budget" sheetId="1" r:id="rId1"/>
@@ -24,15 +24,15 @@
     <sheet name="QRODES" sheetId="13" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'01-Budget'!$A$2:$A$38</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'01-Budget'!$D$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'01-Budget'!$D$2:$D$38</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'01-Budget'!$D$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'01-Budget'!$A$2:$A$38</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'01-Budget'!$D$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'01-Budget'!$D$2:$D$38</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'01-Budget'!$C$1</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'01-Budget'!$C$2:$C$38</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'01-Budget'!$D$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'01-Budget'!$C$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="257">
   <si>
     <t>مارس 22</t>
   </si>
@@ -865,6 +865,12 @@
   </si>
   <si>
     <t>GAMM</t>
+  </si>
+  <si>
+    <t>Modes Text</t>
+  </si>
+  <si>
+    <t>We Are expecting the Most frequent monthly income</t>
   </si>
 </sst>
 </file>
@@ -1055,76 +1061,6 @@
   </cellStyles>
   <dxfs count="87">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1231,6 +1167,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="22" formatCode="mmm\-yy"/>
     </dxf>
     <dxf>
@@ -1258,6 +1204,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1277,6 +1233,16 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1424,6 +1390,46 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4759,7 +4765,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4797,7 +4803,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28DE00F0-E062-47DF-BC28-56E70402E63A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>Bank_Balance</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4831,10 +4837,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4872,7 +4878,7 @@
         <cx:series layoutId="treemap" uniqueId="{6662CFD2-F4E4-44DF-9877-43AE9A1B9391}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4896,7 +4902,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4934,7 +4940,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1BFF31CA-FF0B-4B66-8E8E-23B0AA9833CE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -11537,13 +11543,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>3419476</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1000125</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>704849</xdr:rowOff>
+      <xdr:rowOff>695325</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11683,6 +11689,59 @@
         <a:xfrm>
           <a:off x="3429000" y="4318906"/>
           <a:ext cx="971550" cy="812347"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1009649</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>695325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A5665F-E242-40F6-99AB-BEA18BFF6F82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{837473B0-CC2E-450A-ABE3-18F120FF3D39}">
+              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" r:id="rId8"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="2571750"/>
+          <a:ext cx="1009649" cy="695325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13417,7 +13476,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:W38" totalsRowCount="1" headerRowDxfId="86" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:W38" totalsRowCount="1" headerRowDxfId="82" dataDxfId="81">
   <autoFilter ref="A1:W37" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}">
     <filterColumn colId="3">
       <filters>
@@ -13426,33 +13485,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="23">
-    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="84" totalsRowDxfId="83"/>
-    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="80" totalsRowDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="76" totalsRowDxfId="75">
+    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="80" totalsRowDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="72" totalsRowDxfId="71">
       <calculatedColumnFormula>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="56" totalsRowDxfId="55">
+    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="52" totalsRowDxfId="51">
       <calculatedColumnFormula>-1500*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="40" totalsRowDxfId="39">
+    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="36" totalsRowDxfId="35">
       <calculatedColumnFormula>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13461,13 +13520,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:D65" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="28">
       <calculatedColumnFormula>(C2-C1)/C1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13476,22 +13535,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:F14" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:BV4" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}"/>
   <tableColumns count="74">
     <tableColumn id="1" xr3:uid="{BDE661C0-CE9A-43B6-9DB0-D0E627A191B5}" name="Item"/>
@@ -13574,26 +13633,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:E36" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C9" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13896,19 +13955,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1BF799-B63A-49DC-A527-F22F0BF78544}">
-  <dimension ref="A1:W46"/>
+  <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
@@ -16324,37 +16384,47 @@
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C44" s="22" t="s">
+      <c r="A44" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="D44">
-        <f t="array" ref="D44:D46">_xlfn.MODE.MULT(D2:D37)</f>
+      <c r="B44">
+        <f t="array" ref="B44:B46">_xlfn.MODE.MULT(D2:D37)</f>
         <v>40000</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D45">
+      <c r="B45">
         <v>45000</v>
       </c>
+      <c r="E45" s="22"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D46" t="e">
+      <c r="B46" t="e">
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="B47" t="str">
+        <f>CONCATENATE(B44,",",B45)</f>
+        <v>40000,45000</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E2:E38 H2:V38 F2:G5 F6 F7:G22">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W37">
-    <cfRule type="top10" dxfId="5" priority="12" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="4" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="85" priority="12" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="84" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17407,7 +17477,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E37 C69:D69">
-    <cfRule type="cellIs" dxfId="2" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="18" operator="greaterThan">
       <formula>$C$67*0.03</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17597,7 +17667,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -18762,13 +18832,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A70CCAC-CDEF-4238-8360-E65673389098}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18876,8 +18946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2AF756D-43EE-4B93-A1AF-4696439E3974}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19002,9 +19072,9 @@
       <c r="B8" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C8" s="1">
-        <f>_xlfn.MODE.MULT((Budget_Table[Revenue]))</f>
-        <v>40000</v>
+      <c r="C8" s="1" t="str">
+        <f>'01-Budget'!B47</f>
+        <v>40000,45000</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>192</v>
@@ -19526,7 +19596,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D28:D31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19683,7 +19753,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19714,15 +19784,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="str">
-        <f>CONCATENATE("We Are Expecting to have 
-",TEXT(Budget_Table[[#Totals],[Revenue]],"0.0")," As Monthly Revenue")</f>
-        <v>We Are Expecting to have 
-40000.0 As Monthly Revenue</v>
-      </c>
-      <c r="B3" s="12">
-        <f>Budget_Table[[#Totals],[Revenue]]</f>
-        <v>40000</v>
+      <c r="A3" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="12" t="str">
+        <f>'01-Budget'!B47</f>
+        <v>40000,45000</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
@@ -19768,7 +19835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34094E24-20AA-4501-A8E3-25EFF8D9BA78}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding Barcode Model and Notebook
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yousif Ennwa\Documents\GitHub\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD4AEBD-9755-4312-A72B-ACF200A40753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECB7D04-620F-40C2-9F22-AF88BB22CE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="4" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="5" activeTab="9" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Budget" sheetId="1" r:id="rId1"/>
@@ -22,23 +22,24 @@
     <sheet name="07-Visualization" sheetId="3" r:id="rId7"/>
     <sheet name="08-Story_Telling" sheetId="8" r:id="rId8"/>
     <sheet name="QRODES" sheetId="13" r:id="rId9"/>
+    <sheet name="QRDATASOURCE" sheetId="14" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'01-Budget'!$D$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'01-Budget'!$A$2:$A$38</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'01-Budget'!$D$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'01-Budget'!$D$2:$D$38</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'01-Budget'!$C$2:$C$38</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'01-Budget'!$C$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'01-Budget'!$C$2:$C$38</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'01-Budget'!$A$2:$A$38</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'01-Budget'!$D$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'01-Budget'!$D$2:$D$38</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'01-Budget'!$C$1</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
     <pivotCache cacheId="1" r:id="rId11"/>
     <pivotCache cacheId="2" r:id="rId12"/>
+    <pivotCache cacheId="3" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -93,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="257">
   <si>
     <t>مارس 22</t>
   </si>
@@ -1059,7 +1060,22 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="92">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4695,7 +4711,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4733,7 +4749,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{F2DA8020-A2E8-42D1-B4D9-579780C22758}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Bank_Balance</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4837,10 +4853,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4878,7 +4894,7 @@
         <cx:series layoutId="treemap" uniqueId="{6662CFD2-F4E4-44DF-9877-43AE9A1B9391}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13237,7 +13253,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3CB945B-5FBB-47B3-8AB6-20274BB6CA56}" name="PivotTable14" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3CB945B-5FBB-47B3-8AB6-20274BB6CA56}" name="PivotTable14" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A2:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="23">
     <pivotField axis="axisRow" showAll="0">
@@ -13370,7 +13386,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4CAE920-1561-4824-B4C7-56E973E3D6B2}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4CAE920-1561-4824-B4C7-56E973E3D6B2}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A10:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13415,7 +13431,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D3925E7-8F73-44B0-9992-21F1E0B1CFAF}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D3925E7-8F73-44B0-9992-21F1E0B1CFAF}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A40:B47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13476,7 +13492,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:W38" totalsRowCount="1" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:W38" totalsRowCount="1" headerRowDxfId="87" dataDxfId="86">
   <autoFilter ref="A1:W37" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}">
     <filterColumn colId="3">
       <filters>
@@ -13485,33 +13501,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="23">
-    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="80" totalsRowDxfId="79"/>
-    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="72" totalsRowDxfId="71">
+    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="77" totalsRowDxfId="76">
       <calculatedColumnFormula>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="52" totalsRowDxfId="51">
+    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula>-1500*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="36" totalsRowDxfId="35">
+    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="41" totalsRowDxfId="40">
       <calculatedColumnFormula>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13520,13 +13536,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A1:D65" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="33">
       <calculatedColumnFormula>(C2-C1)/C1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13535,22 +13551,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:F14" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A1:BV4" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}"/>
   <tableColumns count="74">
     <tableColumn id="1" xr3:uid="{BDE661C0-CE9A-43B6-9DB0-D0E627A191B5}" name="Item"/>
@@ -13633,26 +13649,38 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:E36" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:C9" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}" name="Table68" displayName="Table68" ref="A1:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C9" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0323F7C7-1DB8-4F54-8866-477BCC7ACE27}" name="Year" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{1D0671B4-9EF9-4F75-8B21-941CC74796EE}" name="Generated" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B9BDCF29-410A-480C-B445-F5D7C354BB0F}" name="Usage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16415,16 +16443,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E2:E38 H2:V38 F2:G5 F6 F7:G22">
-    <cfRule type="cellIs" dxfId="86" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W37">
-    <cfRule type="top10" dxfId="85" priority="12" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="84" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="90" priority="12" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="89" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="cellIs" dxfId="83" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16433,6 +16461,125 @@
   <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C9CCB2-B26D-49E2-B6BA-121925740299}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C2" s="1">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3300</v>
+      </c>
+      <c r="C4" s="1">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8800</v>
+      </c>
+      <c r="C8" s="1">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="1">
+        <f>_xlfn.FORECAST.LINEAR(Table68[[#This Row],[Year]],B2:B8,A2:A8)</f>
+        <v>13150</v>
+      </c>
+      <c r="C9" s="1">
+        <f>_xlfn.FORECAST.LINEAR(Table68[[#This Row],[Year]],C2:C8,A2:A8)</f>
+        <v>0.92857142857974395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -17477,7 +17624,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E37 C69:D69">
-    <cfRule type="cellIs" dxfId="34" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="18" operator="greaterThan">
       <formula>$C$67*0.03</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17667,7 +17814,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -18832,7 +18979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A70CCAC-CDEF-4238-8360-E65673389098}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -19596,7 +19743,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D28:D31">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19836,7 +19983,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding Matrix in pivot table with apply function to generate new attribute
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yousif Ennwa\Documents\GitHub\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECB7D04-620F-40C2-9F22-AF88BB22CE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F71C8C-8EAC-4BA2-9518-524FA81D4EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="5" activeTab="9" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Budget" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,21 @@
     <sheet name="QRDATASOURCE" sheetId="14" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'01-Budget'!$D$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'01-Budget'!$C$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'01-Budget'!$C$2:$C$38</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'01-Budget'!$C$2:$C$38</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'01-Budget'!$A$2:$A$38</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'01-Budget'!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'01-Budget'!$D$2:$D$38</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'01-Budget'!$D$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'01-Budget'!$A$2:$A$38</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'01-Budget'!$D$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'01-Budget'!$D$2:$D$38</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId11"/>
-    <pivotCache cacheId="2" r:id="rId12"/>
-    <pivotCache cacheId="3" r:id="rId13"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="2" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1092,6 +1092,75 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1261,34 +1330,7 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1344,49 +1386,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1584,24 +1584,114 @@
             <c:strRef>
               <c:f>'01-Budget'!$B$2:$B$37</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>مارس 22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>إبريل 22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>مايو 22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>يونيو 22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>يوليو 22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>أغسطس 22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>سبتمبر 22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>أكتوبر 22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>نوفمبر 22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ديسمبر 22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>يناير 23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>فبراير 23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>مارس 23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>إبريل 23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>مايو 23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>يونيو 23</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>يوليو 23</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>أغسطس 23</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
+                  <c:v>سبتمبر 23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>أكتوبر 23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>نوفمبر 23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>ديسمبر 23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>يناير 24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>فبراير 24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>مارس 24</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>إبريل 24</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="26">
                   <c:v>مايو 24</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="27">
                   <c:v>يونيو 24</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="28">
                   <c:v>يوليو 24</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="29">
                   <c:v>أغسطس 24</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>سبتمبر 24</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>أكتوبر 24</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>نوفمبر 24</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>ديسمبر 24</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>يناير 25</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>فبراير 25</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1611,24 +1701,114 @@
               <c:f>'01-Budget'!$C$2:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83050</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91240</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89290</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>102910</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71260</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60810</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100060</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>119110</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>115250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>124300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92850</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>98900</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>92450</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>107500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>102550</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>112600</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
+                  <c:v>68550</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>101350</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>127950</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>110050</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>122100</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>103650</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>117700</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="26">
                   <c:v>114850</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="27">
                   <c:v>136500</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="28">
                   <c:v>138150</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="29">
                   <c:v>151800</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>107750</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>99300</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>142530</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>169130</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>171230</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>177830</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2353,7 +2533,7 @@
         <c:idx val="13"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="accent2"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2371,7 +2551,7 @@
         <c:idx val="14"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="accent3"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2389,7 +2569,7 @@
         <c:idx val="15"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="accent4"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2901,24 +3081,114 @@
               <c:f>'01-Budget'!$A$2:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2023</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>2024</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="23">
                   <c:v>2024</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="24">
                   <c:v>2024</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="25">
                   <c:v>2024</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
                   <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2928,24 +3198,114 @@
               <c:f>'01-Budget'!$D$2:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="26">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="27">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="28">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="29">
                   <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>82000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3244,7 +3604,7 @@
               <c:f>'01-Budget'!$B$2:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3261,6 +3621,96 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3310,24 +3760,114 @@
               <c:f>'01-Budget'!$D$2:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="26">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="27">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="28">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="29">
                   <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>82000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3376,24 +3916,114 @@
               <c:f>'01-Budget'!$W$2:$W$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>83050</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91240</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89290</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102910</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71260</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60810</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100060</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>119110</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>115250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>124300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92850</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>98900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92450</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>107500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>102550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>112600</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>68550</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
+                  <c:v>60100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>101350</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>127950</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110050</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>122100</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>103650</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>117700</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>114850</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="26">
                   <c:v>136500</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="27">
                   <c:v>138150</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="28">
                   <c:v>151800</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="29">
                   <c:v>107750</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>99300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>142530</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>169130</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>171230</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>177830</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>184430</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4711,7 +5341,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4749,7 +5379,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{F2DA8020-A2E8-42D1-B4D9-579780C22758}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Bank_Balance</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4781,7 +5411,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4819,7 +5449,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28DE00F0-E062-47DF-BC28-56E70402E63A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Bank_Balance</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4853,10 +5483,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4894,7 +5524,7 @@
         <cx:series layoutId="treemap" uniqueId="{6662CFD2-F4E4-44DF-9877-43AE9A1B9391}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4918,7 +5548,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4956,7 +5586,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1BFF31CA-FF0B-4B66-8E8E-23B0AA9833CE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13253,7 +13883,52 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3CB945B-5FBB-47B3-8AB6-20274BB6CA56}" name="PivotTable14" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4CAE920-1561-4824-B4C7-56E973E3D6B2}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A10:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Item_Val" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3CB945B-5FBB-47B3-8AB6-20274BB6CA56}" name="PivotTable14" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A2:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="23">
     <pivotField axis="axisRow" showAll="0">
@@ -13385,53 +14060,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4CAE920-1561-4824-B4C7-56E973E3D6B2}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A10:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Item_Val" fld="1" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D3925E7-8F73-44B0-9992-21F1E0B1CFAF}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D3925E7-8F73-44B0-9992-21F1E0B1CFAF}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A40:B47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13493,41 +14123,35 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:W38" totalsRowCount="1" headerRowDxfId="87" dataDxfId="86">
-  <autoFilter ref="A1:W37" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="40000"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:W37" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}"/>
   <tableColumns count="23">
-    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="85" totalsRowDxfId="84"/>
-    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="83" totalsRowDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="77" totalsRowDxfId="76">
+    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="85" totalsRowDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="84" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="83" totalsRowDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="82" totalsRowDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="81" totalsRowDxfId="18">
       <calculatedColumnFormula>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="57" totalsRowDxfId="56">
+    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="80" totalsRowDxfId="17"/>
+    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="79" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="77" totalsRowDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="75" totalsRowDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="74" totalsRowDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="73" totalsRowDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="72" totalsRowDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="71" totalsRowDxfId="8">
       <calculatedColumnFormula>-1500*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="41" totalsRowDxfId="40">
+    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="70" totalsRowDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="65" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="63" totalsRowDxfId="0">
       <calculatedColumnFormula>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13536,13 +14160,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:D65" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="56">
       <calculatedColumnFormula>(C2-C1)/C1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13551,22 +14175,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:F14" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="A1:BV4" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}"/>
   <tableColumns count="74">
     <tableColumn id="1" xr3:uid="{BDE661C0-CE9A-43B6-9DB0-D0E627A191B5}" name="Item"/>
@@ -13649,38 +14273,38 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A1:E36" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="34" totalsRowDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:C9" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}" name="Table68" displayName="Table68" ref="A1:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}" name="Table68" displayName="Table68" ref="A1:C9" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:C9" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0323F7C7-1DB8-4F54-8866-477BCC7ACE27}" name="Year" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{1D0671B4-9EF9-4F75-8B21-941CC74796EE}" name="Generated" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{B9BDCF29-410A-480C-B445-F5D7C354BB0F}" name="Usage" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0323F7C7-1DB8-4F54-8866-477BCC7ACE27}" name="Year" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{1D0671B4-9EF9-4F75-8B21-941CC74796EE}" name="Generated" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{B9BDCF29-410A-480C-B445-F5D7C354BB0F}" name="Usage" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13985,8 +14609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1BF799-B63A-49DC-A527-F22F0BF78544}">
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14078,7 +14702,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2022</v>
       </c>
@@ -14139,7 +14763,7 @@
         <v>83050</v>
       </c>
     </row>
-    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2022</v>
       </c>
@@ -14206,7 +14830,7 @@
         <v>71600</v>
       </c>
     </row>
-    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2022</v>
       </c>
@@ -14268,7 +14892,7 @@
         <v>91240</v>
       </c>
     </row>
-    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2022</v>
       </c>
@@ -14332,7 +14956,7 @@
         <v>89290</v>
       </c>
     </row>
-    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2022</v>
       </c>
@@ -14396,7 +15020,7 @@
         <v>102910</v>
       </c>
     </row>
-    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2022</v>
       </c>
@@ -14467,7 +15091,7 @@
         <v>71260</v>
       </c>
     </row>
-    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2022</v>
       </c>
@@ -14529,7 +15153,7 @@
         <v>60810</v>
       </c>
     </row>
-    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2022</v>
       </c>
@@ -14591,7 +15215,7 @@
         <v>100060</v>
       </c>
     </row>
-    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2022</v>
       </c>
@@ -14651,7 +15275,7 @@
         <v>119110</v>
       </c>
     </row>
-    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2022</v>
       </c>
@@ -14716,7 +15340,7 @@
         <v>115250</v>
       </c>
     </row>
-    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2023</v>
       </c>
@@ -14776,7 +15400,7 @@
         <v>124300</v>
       </c>
     </row>
-    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2023</v>
       </c>
@@ -14840,7 +15464,7 @@
         <v>92850</v>
       </c>
     </row>
-    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2023</v>
       </c>
@@ -14902,7 +15526,7 @@
         <v>98900</v>
       </c>
     </row>
-    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
@@ -14967,7 +15591,7 @@
         <v>92450</v>
       </c>
     </row>
-    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
@@ -15027,7 +15651,7 @@
         <v>107500</v>
       </c>
     </row>
-    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -15089,7 +15713,7 @@
         <v>102550</v>
       </c>
     </row>
-    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -15218,7 +15842,7 @@
         <v>68550</v>
       </c>
     </row>
-    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -15280,7 +15904,7 @@
         <v>60100</v>
       </c>
     </row>
-    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -15342,7 +15966,7 @@
         <v>101350</v>
       </c>
     </row>
-    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -15402,7 +16026,7 @@
         <v>127950</v>
       </c>
     </row>
-    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -15467,7 +16091,7 @@
         <v>110050</v>
       </c>
     </row>
-    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2024</v>
       </c>
@@ -15527,7 +16151,7 @@
         <v>122100</v>
       </c>
     </row>
-    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2024</v>
       </c>
@@ -15591,7 +16215,7 @@
         <v>103650</v>
       </c>
     </row>
-    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2024</v>
       </c>
@@ -15969,7 +16593,7 @@
         <v>107750</v>
       </c>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2024</v>
       </c>
@@ -16031,7 +16655,7 @@
         <v>99300</v>
       </c>
     </row>
-    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2024</v>
       </c>
@@ -16093,7 +16717,7 @@
         <v>142530</v>
       </c>
     </row>
-    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2024</v>
       </c>
@@ -16153,7 +16777,7 @@
         <v>169130</v>
       </c>
     </row>
-    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2024</v>
       </c>
@@ -16218,7 +16842,7 @@
         <v>171230</v>
       </c>
     </row>
-    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2025</v>
       </c>
@@ -16278,7 +16902,7 @@
         <v>177830</v>
       </c>
     </row>
-    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2025</v>
       </c>
@@ -16342,37 +16966,37 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1">
         <f>SUBTOTAL(103,Budget_Table[Month])</f>
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C38" s="1">
         <f>SUBTOTAL(104,Budget_Table[Bank_Balance])</f>
-        <v>151800</v>
+        <v>177830</v>
       </c>
       <c r="D38" s="1">
         <f>SUBTOTAL(101,Budget_Table[Revenue])</f>
-        <v>40000</v>
+        <v>44055.555555555555</v>
       </c>
       <c r="E38" s="1">
         <f>SUBTOTAL(101,Budget_Table[Bonus])</f>
-        <v>-400</v>
+        <v>-313.05555555555554</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Salaries])</f>
-        <v>-27000</v>
+        <v>-152000</v>
       </c>
       <c r="I38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Maint])</f>
-        <v>-1200</v>
+        <v>-7200</v>
       </c>
       <c r="J38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Stock])</f>
-        <v>-160000</v>
+        <v>-530000</v>
       </c>
       <c r="K38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Home_Expenses])</f>
-        <v>-60000</v>
+        <v>-363500</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -16383,32 +17007,32 @@
       </c>
       <c r="P38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Schools])</f>
-        <v>0</v>
+        <v>-188000</v>
       </c>
       <c r="Q38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Education])</f>
-        <v>0</v>
+        <v>-36000</v>
       </c>
       <c r="R38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Internet])</f>
-        <v>-3000</v>
+        <v>-17750</v>
       </c>
       <c r="S38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Electric])</f>
-        <v>-6000</v>
+        <v>-35400</v>
       </c>
       <c r="T38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Gas])</f>
-        <v>-600</v>
+        <v>-3600</v>
       </c>
       <c r="U38" s="1"/>
       <c r="V38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Fuel])</f>
-        <v>-4500</v>
+        <v>-26850</v>
       </c>
       <c r="W38" s="1">
         <f>SUBTOTAL(104,Budget_Table[Balance])</f>
-        <v>151800</v>
+        <v>184430</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -16469,7 +17093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C9CCB2-B26D-49E2-B6BA-121925740299}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -17624,7 +18248,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E37 C69:D69">
-    <cfRule type="cellIs" dxfId="39" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="18" operator="greaterThan">
       <formula>$C$67*0.03</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17814,7 +18438,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -19581,11 +20205,11 @@
       </c>
       <c r="C32">
         <f>Budget_Table[[#Totals],[Revenue]]-_xlfn.STDEV.P(Budget_Table[Revenue])</f>
-        <v>27657.785980077148</v>
+        <v>31713.341535632702</v>
       </c>
       <c r="D32" s="1">
         <f>Budget_Table[[#Totals],[Revenue]]+_xlfn.STDEV.P(Budget_Table[Revenue])</f>
-        <v>52342.214019922852</v>
+        <v>56397.769575478407</v>
       </c>
       <c r="E32" s="1"/>
     </row>
@@ -19598,11 +20222,11 @@
       </c>
       <c r="C33">
         <f>Budget_Table[[#Totals],[Revenue]]-2*_xlfn.STDEV.P(Budget_Table[Revenue])</f>
-        <v>15315.571960154295</v>
+        <v>19371.12751570985</v>
       </c>
       <c r="D33" s="1">
         <f>Budget_Table[[#Totals],[Revenue]]+2*_xlfn.STDEV.P(Budget_Table[Revenue])</f>
-        <v>64684.428039845705</v>
+        <v>68739.983595401252</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -19615,11 +20239,11 @@
       </c>
       <c r="C34">
         <f>Budget_Table[[#Totals],[Revenue]]-3*_xlfn.STDEV.P(Budget_Table[Revenue])</f>
-        <v>2973.3579402314426</v>
+        <v>7028.9134957869974</v>
       </c>
       <c r="D34" s="1">
         <f>Budget_Table[[#Totals],[Revenue]]+3*_xlfn.STDEV.P(Budget_Table[Revenue])</f>
-        <v>77026.64205976855</v>
+        <v>81082.197615324112</v>
       </c>
       <c r="E34" s="1"/>
     </row>
@@ -19743,7 +20367,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D28:D31">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update data measurements sessions
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yousif Ennwa\Documents\GitHub\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56968B1A-CE39-473E-B027-F0091CD62651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA315EB-6ED3-45D2-98C5-155134967828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="6" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="5" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Budget" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,7 @@
     <pivotCache cacheId="1" r:id="rId13"/>
     <pivotCache cacheId="2" r:id="rId14"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1112,76 +1113,6 @@
   </cellStyles>
   <dxfs count="99">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1324,6 +1255,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="22" formatCode="mmm\-yy"/>
     </dxf>
     <dxf>
@@ -1351,6 +1292,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1370,6 +1321,16 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1517,6 +1478,46 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -14193,36 +14194,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:W38" totalsRowCount="1" headerRowDxfId="98" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:W38" totalsRowCount="1" headerRowDxfId="94" dataDxfId="93">
   <autoFilter ref="A1:W37" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}"/>
   <tableColumns count="23">
-    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="96" totalsRowDxfId="95"/>
-    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="94" totalsRowDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="92" totalsRowDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="90" totalsRowDxfId="89"/>
-    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="88" totalsRowDxfId="87">
+    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="92" totalsRowDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="90" totalsRowDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="88" totalsRowDxfId="87"/>
+    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="86" totalsRowDxfId="85"/>
+    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="84" totalsRowDxfId="83">
       <calculatedColumnFormula>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="86" totalsRowDxfId="85"/>
-    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="84" totalsRowDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79"/>
-    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="68" totalsRowDxfId="67">
+    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="82" totalsRowDxfId="81"/>
+    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="80" totalsRowDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="72" totalsRowDxfId="71"/>
+    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="64" totalsRowDxfId="63">
       <calculatedColumnFormula>-1500*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="52" totalsRowDxfId="51">
+    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="48" totalsRowDxfId="47">
       <calculatedColumnFormula>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14231,13 +14232,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A1:D65" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="40">
       <calculatedColumnFormula>(C2-C1)/C1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14246,22 +14247,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A1:F14" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="30">
   <autoFilter ref="A1:BV4" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}"/>
   <tableColumns count="74">
     <tableColumn id="1" xr3:uid="{BDE661C0-CE9A-43B6-9DB0-D0E627A191B5}" name="Item"/>
@@ -14344,49 +14345,49 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:E36" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="18" totalsRowDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1D6AD1AE-8BFB-43FE-A342-FAAED5606F39}" name="CVTable" displayName="CVTable" ref="B1:C5" totalsRowCount="1" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1D6AD1AE-8BFB-43FE-A342-FAAED5606F39}" name="CVTable" displayName="CVTable" ref="B1:C5" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14">
   <autoFilter ref="B1:C4" xr:uid="{1D6AD1AE-8BFB-43FE-A342-FAAED5606F39}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EEEA92C2-FCB5-4646-B2D8-21325C961E6C}" name="Doctors" totalsRowFunction="average" dataDxfId="9" totalsRowDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{660608BD-9486-4261-BAE1-13E9696E5733}" name="Teachers" totalsRowFunction="average" dataDxfId="7" totalsRowDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{EEEA92C2-FCB5-4646-B2D8-21325C961E6C}" name="Doctors" totalsRowFunction="average" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{660608BD-9486-4261-BAE1-13E9696E5733}" name="Teachers" totalsRowFunction="average" dataDxfId="11" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:C9" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}" name="Table68" displayName="Table68" ref="A1:C9" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}" name="Table68" displayName="Table68" ref="A1:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C9" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0323F7C7-1DB8-4F54-8866-477BCC7ACE27}" name="Year" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{1D0671B4-9EF9-4F75-8B21-941CC74796EE}" name="Generated" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{B9BDCF29-410A-480C-B445-F5D7C354BB0F}" name="Usage" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{0323F7C7-1DB8-4F54-8866-477BCC7ACE27}" name="Year" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{1D0671B4-9EF9-4F75-8B21-941CC74796EE}" name="Generated" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{B9BDCF29-410A-480C-B445-F5D7C354BB0F}" name="Usage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14692,7 +14693,7 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD49"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17149,16 +17150,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E2:E38 H2:V38 F2:G5 F6 F7:G22">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W37">
-    <cfRule type="top10" dxfId="5" priority="12" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="4" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="97" priority="12" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="96" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17481,8 +17482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22144E8-9C70-4018-BA08-A3D7E2B79E76}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18517,7 +18518,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E37 C69:D69">
-    <cfRule type="cellIs" dxfId="2" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="18" operator="greaterThan">
       <formula>$C$67*0.03</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18707,7 +18708,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -19986,8 +19987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2AF756D-43EE-4B93-A1AF-4696439E3974}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:D37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20636,7 +20637,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D28:D31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20652,7 +20653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBF5096-32F4-47AD-9929-FBFB46D1C4A6}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update for adding heatmap color map
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yousif Ennwa\Documents\GitHub\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A546C94-30A2-4358-9CFE-569A47A66B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4E693E-1A82-48F9-9D36-C5AF26102468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="4" activeTab="7" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3EC47B49-2BAD-4354-82B7-F4FC7A092D12}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Budget" sheetId="1" r:id="rId1"/>
@@ -26,32 +26,21 @@
     <sheet name="QRDATASOURCE" sheetId="14" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'01-Budget'!$A$1:$A$37</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'01-Budget'!$A$2:$A$38</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'01-Budget'!$B$1:$B$37</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'01-Budget'!$D$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'01-Budget'!$D$2:$D$38</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'01-Budget'!$D$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'01-Budget'!$C$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'01-Budget'!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'01-Budget'!$E$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'01-Budget'!$E$2:$E$37</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'01-Budget'!$D$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'01-Budget'!$D$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'01-Budget'!$D$2:$D$37</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'01-Budget'!$B$1:$B$37</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'01-Budget'!$E$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'01-Budget'!$E$2:$E$38</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId12"/>
-    <pivotCache cacheId="2" r:id="rId13"/>
-    <pivotCache cacheId="3" r:id="rId14"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="2" r:id="rId14"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -75,7 +64,7 @@
     <author>Yousif Ennwa</author>
   </authors>
   <commentList>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{80C00E00-3D60-457A-A74B-CA6357091704}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{80C00E00-3D60-457A-A74B-CA6357091704}">
       <text>
         <r>
           <rPr>
@@ -106,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="278">
   <si>
     <t>مارس 22</t>
   </si>
@@ -908,6 +897,45 @@
   </si>
   <si>
     <t>Group 03</t>
+  </si>
+  <si>
+    <t>MonthE</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Novmber</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1149,82 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="101">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1383,34 +1486,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1466,49 +1542,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1635,7 +1669,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Budget'!$C$1</c:f>
+              <c:f>'01-Budget'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1780,7 +1814,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'01-Budget'!$C$2:$C$37</c:f>
+              <c:f>'01-Budget'!$D$2:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -3113,7 +3147,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Budget'!$D$1</c:f>
+              <c:f>'01-Budget'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3277,7 +3311,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'01-Budget'!$D$2:$D$38</c:f>
+              <c:f>'01-Budget'!$E$2:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -3810,7 +3844,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Budget'!$D$1</c:f>
+              <c:f>'01-Budget'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3839,7 +3873,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'01-Budget'!$D$2:$D$38</c:f>
+              <c:f>'01-Budget'!$E$2:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -3966,7 +4000,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Budget'!$W$1</c:f>
+              <c:f>'01-Budget'!$X$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3995,7 +4029,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'01-Budget'!$W$2:$W$38</c:f>
+              <c:f>'01-Budget'!$X$2:$X$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -4404,7 +4438,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Budget'!$C$1</c:f>
+              <c:f>'01-Budget'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4425,7 +4459,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'01-Budget'!$C$2:$C$37</c:f>
+              <c:f>'01-Budget'!$D$2:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -5256,7 +5290,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5294,7 +5328,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28DE00F0-E062-47DF-BC28-56E70402E63A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Bank_Balance</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5328,10 +5362,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5369,7 +5403,7 @@
         <cx:series layoutId="treemap" uniqueId="{6662CFD2-F4E4-44DF-9877-43AE9A1B9391}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5393,7 +5427,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5431,7 +5465,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1BFF31CA-FF0B-4B66-8E8E-23B0AA9833CE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5465,7 +5499,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5503,7 +5537,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{AB15F118-9EEC-4D53-8944-F0A2911CD900}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Bank_Balance</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13675,7 +13709,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4CAE920-1561-4824-B4C7-56E973E3D6B2}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4CAE920-1561-4824-B4C7-56E973E3D6B2}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A10:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13720,7 +13754,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3CB945B-5FBB-47B3-8AB6-20274BB6CA56}" name="PivotTable14" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3CB945B-5FBB-47B3-8AB6-20274BB6CA56}" name="PivotTable14" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A2:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="23">
     <pivotField axis="axisRow" showAll="0">
@@ -13853,7 +13887,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D3925E7-8F73-44B0-9992-21F1E0B1CFAF}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D3925E7-8F73-44B0-9992-21F1E0B1CFAF}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A40:B47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13914,36 +13948,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:W38" totalsRowCount="1" headerRowDxfId="98" dataDxfId="97">
-  <autoFilter ref="A1:W37" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}"/>
-  <tableColumns count="23">
-    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="96" totalsRowDxfId="95"/>
-    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="94" totalsRowDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="92" totalsRowDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="90" totalsRowDxfId="89"/>
-    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="88" totalsRowDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}" name="Budget_Table" displayName="Budget_Table" ref="A1:X38" totalsRowCount="1" headerRowDxfId="100" dataDxfId="99">
+  <autoFilter ref="A1:X37" xr:uid="{3312BD19-C58D-44C9-9081-35E47D6BEE91}"/>
+  <tableColumns count="24">
+    <tableColumn id="24" xr3:uid="{F923AF45-9D46-4D18-B925-38B8BEB86059}" name="Year" dataDxfId="98" totalsRowDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{8EBBE7C2-C046-4B4A-B640-ED5DBC962B6F}" name="Month" totalsRowFunction="count" dataDxfId="97" totalsRowDxfId="22"/>
+    <tableColumn id="20" xr3:uid="{D1C7EAB1-8A5D-460B-B0C1-37BDFD80F1C1}" name="MonthE" dataDxfId="24" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{8A63691D-8589-42E7-A686-3BD5BB74A8B1}" name="Bank_Balance" totalsRowFunction="max" dataDxfId="96" totalsRowDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{1203E385-0896-49BE-86F3-C5477688602A}" name="Revenue" totalsRowFunction="average" dataDxfId="95" totalsRowDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{508C90CE-22D3-4800-8230-DA9F8D2CA19B}" name="Bonus" totalsRowFunction="average" dataDxfId="94" totalsRowDxfId="18">
       <calculatedColumnFormula>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="86" totalsRowDxfId="85"/>
-    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="84" totalsRowDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79"/>
-    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="68" totalsRowDxfId="67">
+    <tableColumn id="14" xr3:uid="{73A5A091-CE88-421D-B76E-51199219B2B8}" name="Gammiat" dataDxfId="93" totalsRowDxfId="17"/>
+    <tableColumn id="23" xr3:uid="{8B037BAA-9974-45EB-87C6-912132963841}" name="ZAKAT" dataDxfId="92" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4268231F-3502-48F5-9ECC-1EF1B54B200D}" name="Salaries" totalsRowFunction="sum" dataDxfId="91" totalsRowDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{B4D2DED4-25E4-4438-BCAA-3CAEBD7F2E68}" name="Maint" totalsRowFunction="sum" dataDxfId="90" totalsRowDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{66310BEE-AE75-45F0-B222-7003746C065A}" name="Stock" totalsRowFunction="sum" dataDxfId="89" totalsRowDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{0D7FFC00-3FC9-484D-A5E1-85ECA7D816E7}" name="Home_Expenses" totalsRowFunction="sum" dataDxfId="88" totalsRowDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{D0F0DF57-5B43-4740-831F-228734FC7DE7}" name="Cleanind" dataDxfId="87" totalsRowDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{036C41B7-0FB1-43D6-9089-3A790919B056}" name="Medicines" dataDxfId="86" totalsRowDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{6F9E872C-9774-4953-B865-B1AAEEDC7EBB}" name="Club" dataDxfId="85" totalsRowDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{ED175497-748B-40EC-B0AF-DE5405F441D1}" name="Cloths" totalsRowFunction="average" dataDxfId="84" totalsRowDxfId="8">
       <calculatedColumnFormula>-1500*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="52" totalsRowDxfId="51">
+    <tableColumn id="12" xr3:uid="{257E32F4-CFAD-49C5-A482-67A4E94CC271}" name="Schools" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{406538B9-50A6-4920-BC9A-8CFF81111415}" name="Education" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{96F05650-A0B8-48FD-9FF2-0CF2D042920F}" name="Internet" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{95C77D14-0A76-4D03-A378-9A2F9589D3A9}" name="Electric" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{8B1308FF-6556-45E1-B5DF-82DBE6BD17DD}" name="Gas" totalsRowFunction="sum" dataDxfId="79" totalsRowDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{8C97B4B6-F32B-4BEB-96DE-ABF8666A8064}" name="Add_Expenses" dataDxfId="78" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{3232CB77-E33A-4499-B61C-DE4C55BD1427}" name="Fuel" totalsRowFunction="sum" dataDxfId="77" totalsRowDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{49E26DD5-7DCC-4DE2-9A44-D49E5EA1A831}" name="Balance" totalsRowFunction="max" dataDxfId="76" totalsRowDxfId="0">
       <calculatedColumnFormula>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13952,13 +13987,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}" name="Gold_Forecasting" displayName="Gold_Forecasting" ref="A1:D65" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="A1:D65" xr:uid="{C3265939-9DDE-49D0-B16D-992584708B59}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{C1615512-B305-443E-B90D-B937DDC12AAD}" name="Date" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{CD51677C-1FFD-4666-8219-66C9FA06991E}" name="Item" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{0763EF00-2B55-43F7-ABF4-D1736C803D76}" name="Item_Val" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{48268654-5DAF-481F-8F79-BFA62E4DE8CF}" name="Growth" dataDxfId="70">
       <calculatedColumnFormula>(C2-C1)/C1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13967,22 +14002,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}" name="Table5" displayName="Table5" ref="A1:F14" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="A1:F14" xr:uid="{295D201E-D7C4-4A70-B04C-58DAFE9F33CA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{2BB46849-9F9D-4DF6-A2B9-97B67F7EBBCE}" name="Attribute" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{D3B47D54-C984-4A64-81BD-BFB3E291E849}" name="Object" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{C0CFD872-AE2C-4A70-ADCE-553B5A5141BA}" name="Attribute_Desc" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{0414412C-1674-4CB5-BC78-E617BCDAADBC}" name="Question" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{7E7A64D1-692D-49BD-B53A-18EFBB427A10}" name="Answer Approach" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{A422447F-2544-4757-8822-5241B7C0C8B4}" name="Type" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}" name="Table3" displayName="Table3" ref="A1:BV4" totalsRowShown="0" headerRowDxfId="61">
   <autoFilter ref="A1:BV4" xr:uid="{C51C5359-9FAD-4C6C-A48B-ED0F315A7D69}"/>
   <tableColumns count="74">
     <tableColumn id="1" xr3:uid="{BDE661C0-CE9A-43B6-9DB0-D0E627A191B5}" name="Item"/>
@@ -14065,49 +14100,49 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}" name="Measurements_Table" displayName="Measurements_Table" ref="A1:E37" totalsRowCount="1" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A1:E36" xr:uid="{08D949C8-7183-46B8-B8DE-C8500CEA663F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{3DE165E8-C653-49B1-B9FF-7DF40D0C7678}" name="Measurements Types" totalsRowLabel="Count" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{24E7BC82-A5E3-4B02-AB56-BCA40829095C}" name="Measurement" totalsRowFunction="count" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{43D487C5-6DD1-4CBA-8692-C9C781D0BAA9}" name="Value" totalsRowFunction="count" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{E4F9C1FF-E028-4100-B23F-AD155885FE70}" name="Description" totalsRowFunction="count" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{15DB07C0-D3A2-4E9F-8472-87FB97F1E68B}" name="Why We need It" totalsRowFunction="count" dataDxfId="50" totalsRowDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1D6AD1AE-8BFB-43FE-A342-FAAED5606F39}" name="CVTable" displayName="CVTable" ref="B1:C5" totalsRowCount="1" headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1D6AD1AE-8BFB-43FE-A342-FAAED5606F39}" name="CVTable" displayName="CVTable" ref="B1:C5" totalsRowCount="1" headerRowDxfId="48" dataDxfId="47" totalsRowDxfId="46">
   <autoFilter ref="B1:C4" xr:uid="{1D6AD1AE-8BFB-43FE-A342-FAAED5606F39}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EEEA92C2-FCB5-4646-B2D8-21325C961E6C}" name="Doctors" totalsRowFunction="average" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{660608BD-9486-4261-BAE1-13E9696E5733}" name="Teachers" totalsRowFunction="average" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{EEEA92C2-FCB5-4646-B2D8-21325C961E6C}" name="Doctors" totalsRowFunction="average" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{660608BD-9486-4261-BAE1-13E9696E5733}" name="Teachers" totalsRowFunction="average" dataDxfId="43" totalsRowDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:C9" xr:uid="{AE0EDD48-DF6B-42AE-AC77-8C772E5BA9E5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F09306D3-A1F2-41E1-86DC-67EDFBC18722}" name="Year" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{2BC120C4-42A7-4B5F-B780-E61305548892}" name="Generated" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{E28AE0CD-4C45-4B53-BFFA-03DDE4A9CBD4}" name="Usage" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}" name="Table68" displayName="Table68" ref="A1:C9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}" name="Table68" displayName="Table68" ref="A1:C9" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:C9" xr:uid="{77E360E5-2067-40BC-B7A3-06095CBD22CF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0323F7C7-1DB8-4F54-8866-477BCC7ACE27}" name="Year" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{1D0671B4-9EF9-4F75-8B21-941CC74796EE}" name="Generated" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{B9BDCF29-410A-480C-B445-F5D7C354BB0F}" name="Usage" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{0323F7C7-1DB8-4F54-8866-477BCC7ACE27}" name="Year" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{1D0671B4-9EF9-4F75-8B21-941CC74796EE}" name="Generated" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B9BDCF29-410A-480C-B445-F5D7C354BB0F}" name="Usage" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14410,10 +14445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1BF799-B63A-49DC-A527-F22F0BF78544}">
-  <dimension ref="A1:W47"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C37"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14434,7 +14469,7 @@
     <col min="26" max="26" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -14442,2423 +14477,2535 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2022</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="1">
         <v>70000</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>30000</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1">
         <v>-3500</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>-200</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1">
         <v>-6500</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>-400</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>-500</v>
       </c>
-      <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1">
         <v>-3000</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
         <v>-250</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>-400</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>-100</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>-1500</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>-600</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>83050</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2022</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <f>W2</f>
+      <c r="C3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="1">
+        <f>X2</f>
         <v>83050</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>39000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>-4000</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
         <v>-3500</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>-200</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>-20000</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>-12000</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>-400</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>-500</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1">
-        <f t="shared" ref="O3:O35" si="0">-1500*3</f>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P35" si="0">-1500*3</f>
         <v>-4500</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1">
         <v>-3000</v>
       </c>
-      <c r="R3" s="1">
+      <c r="S3" s="1">
         <v>-500</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>-1000</v>
       </c>
-      <c r="T3" s="1">
+      <c r="U3" s="1">
         <v>-100</v>
       </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1">
+      <c r="V3" s="1"/>
+      <c r="W3" s="1">
         <v>-750</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>71600</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2022</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <f t="shared" ref="C4:C37" si="1">W3</f>
+      <c r="C4" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D37" si="1">X3</f>
         <v>71600</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>41000</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-410</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>-4000</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1">
         <v>-3500</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>-200</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1">
         <v>-10000</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>-400</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>-500</v>
       </c>
-      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1">
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1">
         <v>0</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
         <v>-500</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>-1000</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U4" s="1">
         <v>-100</v>
       </c>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1">
+      <c r="V4" s="1"/>
+      <c r="W4" s="1">
         <v>-750</v>
       </c>
-      <c r="W4" s="1">
+      <c r="X4" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>91240</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2022</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
         <v>91240</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>39000</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>-4000</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
         <v>-3500</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>-200</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>-20000</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>-10000</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>-400</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>-500</v>
       </c>
-      <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1">
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1">
         <v>0</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S5" s="1">
         <v>-500</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>-1000</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U5" s="1">
         <v>-100</v>
       </c>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1">
+      <c r="V5" s="1"/>
+      <c r="W5" s="1">
         <v>-750</v>
       </c>
-      <c r="W5" s="1">
+      <c r="X5" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>89290</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2022</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D6" s="1">
         <f t="shared" si="1"/>
         <v>89290</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>43000</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-430</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>-4000</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1">
         <v>-3500</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>-200</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
         <v>-10000</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>-400</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>-500</v>
       </c>
-      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1">
         <v>-8000</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
         <v>0</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
         <v>-500</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <v>-1000</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U6" s="1">
         <v>-100</v>
       </c>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1">
+      <c r="V6" s="1"/>
+      <c r="W6" s="1">
         <v>-750</v>
       </c>
-      <c r="W6" s="1">
+      <c r="X6" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>102910</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2022</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="1">
         <f t="shared" si="1"/>
         <v>102910</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>39000</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>20000</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>-8000</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>-3500</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>-200</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>-60000</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>-10000</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>-400</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>-500</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>-1200</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <f t="shared" si="0"/>
         <v>-4500</v>
       </c>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1">
         <v>0</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>-500</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>-1000</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>-100</v>
       </c>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1">
+      <c r="V7" s="1"/>
+      <c r="W7" s="1">
         <v>-750</v>
       </c>
-      <c r="W7" s="1">
+      <c r="X7" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>71260</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2022</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D8" s="1">
         <f t="shared" si="1"/>
         <v>71260</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>50000</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-500</v>
       </c>
-      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1">
         <v>-3500</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>-200</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1">
         <v>-10000</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>-400</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>-500</v>
       </c>
-      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1">
         <v>-40000</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <v>-3000</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <v>-500</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>-1000</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>-100</v>
       </c>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1">
+      <c r="V8" s="1"/>
+      <c r="W8" s="1">
         <v>-750</v>
       </c>
-      <c r="W8" s="1">
+      <c r="X8" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>60810</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2022</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>60810</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>80000</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-800</v>
       </c>
-      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
         <v>-3500</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>-200</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>-20000</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>-10000</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M9" s="1">
         <v>-400</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>-500</v>
       </c>
-      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1">
         <v>-3000</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9" s="1">
         <v>-500</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <v>-1000</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U9" s="1">
         <v>-100</v>
       </c>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1">
+      <c r="V9" s="1"/>
+      <c r="W9" s="1">
         <v>-750</v>
       </c>
-      <c r="W9" s="1">
+      <c r="X9" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>100060</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2022</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D10" s="1">
         <f t="shared" si="1"/>
         <v>100060</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>39000</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
         <v>-3500</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>-200</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
         <v>-10000</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <v>-400</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>-500</v>
       </c>
-      <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1">
         <v>-3000</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <v>-500</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <v>-1000</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>-100</v>
       </c>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1">
+      <c r="V10" s="1"/>
+      <c r="W10" s="1">
         <v>-750</v>
       </c>
-      <c r="W10" s="1">
+      <c r="X10" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>119110</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2022</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
         <v>119110</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>41000</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-410</v>
       </c>
-      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
         <v>-3500</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>-200</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>-20000</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>-10000</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>-400</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>-500</v>
       </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1">
+      <c r="O11" s="1"/>
+      <c r="P11" s="1">
         <f t="shared" si="0"/>
         <v>-4500</v>
       </c>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1">
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1">
         <v>-3000</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S11" s="1">
         <v>-500</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <v>-1000</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>-100</v>
       </c>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1">
+      <c r="V11" s="1"/>
+      <c r="W11" s="1">
         <v>-750</v>
       </c>
-      <c r="W11" s="1">
+      <c r="X11" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>115250</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>115250</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>30000</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1">
         <v>-4500</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>-200</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
         <v>-10000</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M12" s="1">
         <v>-400</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>-500</v>
       </c>
-      <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="1">
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1">
         <v>-3000</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S12" s="1">
         <v>-500</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <v>-1000</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U12" s="1">
         <v>-100</v>
       </c>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1">
+      <c r="V12" s="1"/>
+      <c r="W12" s="1">
         <v>-750</v>
       </c>
-      <c r="W12" s="1">
+      <c r="X12" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>124300</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>124300</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>50000</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-500</v>
       </c>
-      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1">
         <v>-4500</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>-200</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>-30000</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <v>-10000</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>-400</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>-500</v>
       </c>
-      <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1">
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1">
         <v>-30000</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R13" s="1">
         <v>-3000</v>
       </c>
-      <c r="R13" s="1">
+      <c r="S13" s="1">
         <v>-500</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T13" s="1">
         <v>-1000</v>
       </c>
-      <c r="T13" s="1">
+      <c r="U13" s="1">
         <v>-100</v>
       </c>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1">
+      <c r="V13" s="1"/>
+      <c r="W13" s="1">
         <v>-750</v>
       </c>
-      <c r="W13" s="1">
+      <c r="X13" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>92850</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>92850</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>33000</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1">
         <v>-4500</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>-200</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1">
+      <c r="K14" s="1"/>
+      <c r="L14" s="1">
         <v>-15000</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <v>-400</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>-500</v>
       </c>
-      <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="1">
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1">
         <v>-3000</v>
       </c>
-      <c r="R14" s="1">
+      <c r="S14" s="1">
         <v>-500</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T14" s="1">
         <v>-1000</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U14" s="1">
         <v>-100</v>
       </c>
-      <c r="U14" s="1">
+      <c r="V14" s="1">
         <v>-1000</v>
       </c>
-      <c r="V14" s="1">
+      <c r="W14" s="1">
         <v>-750</v>
       </c>
-      <c r="W14" s="1">
+      <c r="X14" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>98900</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>98900</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>39000</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1">
+      <c r="H15" s="1"/>
+      <c r="I15" s="1">
         <v>-4500</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>-200</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>-20000</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>-10000</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <v>-400</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>-500</v>
       </c>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1">
+      <c r="O15" s="1"/>
+      <c r="P15" s="1">
         <f t="shared" si="0"/>
         <v>-4500</v>
       </c>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1">
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1">
         <v>-3000</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S15" s="1">
         <v>-500</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T15" s="1">
         <v>-1000</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U15" s="1">
         <v>-100</v>
       </c>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1">
+      <c r="V15" s="1"/>
+      <c r="W15" s="1">
         <v>-750</v>
       </c>
-      <c r="W15" s="1">
+      <c r="X15" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>92450</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>92450</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>36000</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1">
         <v>-4500</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>-200</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1">
+      <c r="K16" s="1"/>
+      <c r="L16" s="1">
         <v>-10000</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <v>-400</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>-500</v>
       </c>
-      <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="1">
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1">
         <v>-3000</v>
       </c>
-      <c r="R16" s="1">
+      <c r="S16" s="1">
         <v>-500</v>
       </c>
-      <c r="S16" s="1">
+      <c r="T16" s="1">
         <v>-1000</v>
       </c>
-      <c r="T16" s="1">
+      <c r="U16" s="1">
         <v>-100</v>
       </c>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1">
+      <c r="V16" s="1"/>
+      <c r="W16" s="1">
         <v>-750</v>
       </c>
-      <c r="W16" s="1">
+      <c r="X16" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>107500</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" s="1">
         <f t="shared" si="1"/>
         <v>107500</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>36000</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1">
         <v>-4500</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>-200</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>-20000</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>-10000</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <v>-400</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <v>-500</v>
       </c>
-      <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="1">
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1">
         <v>-3000</v>
       </c>
-      <c r="R17" s="1">
+      <c r="S17" s="1">
         <v>-500</v>
       </c>
-      <c r="S17" s="1">
+      <c r="T17" s="1">
         <v>-1000</v>
       </c>
-      <c r="T17" s="1">
+      <c r="U17" s="1">
         <v>-100</v>
       </c>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1">
+      <c r="V17" s="1"/>
+      <c r="W17" s="1">
         <v>-750</v>
       </c>
-      <c r="W17" s="1">
+      <c r="X17" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>102550</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D18" s="1">
         <f t="shared" si="1"/>
         <v>102550</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>36000</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1">
         <v>-8000</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>-4500</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>-200</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1">
+      <c r="K18" s="1"/>
+      <c r="L18" s="1">
         <v>-10000</v>
       </c>
-      <c r="L18" s="1">
+      <c r="M18" s="1">
         <v>-400</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>-500</v>
       </c>
-      <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="1">
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1">
         <v>0</v>
       </c>
-      <c r="R18" s="1">
+      <c r="S18" s="1">
         <v>-500</v>
       </c>
-      <c r="S18" s="1">
+      <c r="T18" s="1">
         <v>-1000</v>
       </c>
-      <c r="T18" s="1">
+      <c r="U18" s="1">
         <v>-100</v>
       </c>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1">
+      <c r="V18" s="1"/>
+      <c r="W18" s="1">
         <v>-750</v>
       </c>
-      <c r="W18" s="1">
+      <c r="X18" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>112600</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="1">
         <f t="shared" si="1"/>
         <v>112600</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>40000</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-400</v>
       </c>
-      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1">
         <v>-4500</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>-200</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <v>-60000</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>-10000</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <v>-400</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <v>-500</v>
       </c>
-      <c r="N19" s="1">
+      <c r="O19" s="1">
         <v>-1200</v>
       </c>
-      <c r="O19" s="1">
+      <c r="P19" s="1">
         <f t="shared" si="0"/>
         <v>-4500</v>
       </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1">
         <v>0</v>
       </c>
-      <c r="R19" s="1">
+      <c r="S19" s="1">
         <v>-500</v>
       </c>
-      <c r="S19" s="1">
+      <c r="T19" s="1">
         <v>-1000</v>
       </c>
-      <c r="T19" s="1">
+      <c r="U19" s="1">
         <v>-100</v>
       </c>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1">
+      <c r="V19" s="1"/>
+      <c r="W19" s="1">
         <v>-750</v>
       </c>
-      <c r="W19" s="1">
+      <c r="X19" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>68550</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D20" s="1">
         <f t="shared" si="1"/>
         <v>68550</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>50000</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-500</v>
       </c>
-      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1">
         <v>-4500</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>-200</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1">
+      <c r="K20" s="1"/>
+      <c r="L20" s="1">
         <v>-10000</v>
       </c>
-      <c r="L20" s="1">
+      <c r="M20" s="1">
         <v>-400</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <v>-500</v>
       </c>
-      <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="1">
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1">
         <v>-40000</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R20" s="1">
         <v>0</v>
       </c>
-      <c r="R20" s="1">
+      <c r="S20" s="1">
         <v>-500</v>
       </c>
-      <c r="S20" s="1">
+      <c r="T20" s="1">
         <v>-1000</v>
       </c>
-      <c r="T20" s="1">
+      <c r="U20" s="1">
         <v>-100</v>
       </c>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1">
+      <c r="V20" s="1"/>
+      <c r="W20" s="1">
         <v>-750</v>
       </c>
-      <c r="W20" s="1">
+      <c r="X20" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>60100</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D21" s="1">
         <f t="shared" si="1"/>
         <v>60100</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>80000</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-800</v>
       </c>
-      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1">
         <v>-4500</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>-200</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <v>-20000</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <v>-10000</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M21" s="1">
         <v>-400</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>-500</v>
       </c>
-      <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="1">
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1">
         <v>0</v>
       </c>
-      <c r="R21" s="1">
+      <c r="S21" s="1">
         <v>-500</v>
       </c>
-      <c r="S21" s="1">
+      <c r="T21" s="1">
         <v>-1000</v>
       </c>
-      <c r="T21" s="1">
+      <c r="U21" s="1">
         <v>-100</v>
       </c>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1">
+      <c r="V21" s="1"/>
+      <c r="W21" s="1">
         <v>-750</v>
       </c>
-      <c r="W21" s="1">
+      <c r="X21" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>101350</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D22" s="1">
         <f t="shared" si="1"/>
         <v>101350</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>45000</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-450</v>
       </c>
-      <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1">
         <v>-4500</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>-200</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1">
+      <c r="K22" s="1"/>
+      <c r="L22" s="1">
         <v>-10000</v>
       </c>
-      <c r="L22" s="1">
+      <c r="M22" s="1">
         <v>-400</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <v>-500</v>
       </c>
-      <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="1">
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1">
         <v>0</v>
       </c>
-      <c r="R22" s="1">
+      <c r="S22" s="1">
         <v>-500</v>
       </c>
-      <c r="S22" s="1">
+      <c r="T22" s="1">
         <v>-1000</v>
       </c>
-      <c r="T22" s="1">
+      <c r="U22" s="1">
         <v>-100</v>
       </c>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1">
+      <c r="V22" s="1"/>
+      <c r="W22" s="1">
         <v>-750</v>
       </c>
-      <c r="W22" s="1">
+      <c r="X22" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>127950</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D23" s="1">
         <f t="shared" si="1"/>
         <v>127950</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>45000</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-450</v>
       </c>
-      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1">
+      <c r="H23" s="1"/>
+      <c r="I23" s="1">
         <v>-4500</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>-200</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <v>-40000</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
         <v>-10000</v>
       </c>
-      <c r="L23" s="1">
+      <c r="M23" s="1">
         <v>-400</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <v>-500</v>
       </c>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1">
+      <c r="O23" s="1"/>
+      <c r="P23" s="1">
         <f t="shared" si="0"/>
         <v>-4500</v>
       </c>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1">
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1">
         <v>0</v>
       </c>
-      <c r="R23" s="1">
+      <c r="S23" s="1">
         <v>-500</v>
       </c>
-      <c r="S23" s="1">
+      <c r="T23" s="1">
         <v>-1000</v>
       </c>
-      <c r="T23" s="1">
+      <c r="U23" s="1">
         <v>-100</v>
       </c>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1">
+      <c r="V23" s="1"/>
+      <c r="W23" s="1">
         <v>-750</v>
       </c>
-      <c r="W23" s="1">
+      <c r="X23" s="1">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>110050</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2024</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D24" s="1">
         <f t="shared" si="1"/>
         <v>110050</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>30000</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1">
         <v>-4500</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>-200</v>
       </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1">
+      <c r="K24" s="1"/>
+      <c r="L24" s="1">
         <v>-10000</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <v>-400</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <v>-500</v>
       </c>
-      <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="1">
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1">
         <v>0</v>
       </c>
-      <c r="R24" s="1">
+      <c r="S24" s="1">
         <v>-500</v>
       </c>
-      <c r="S24" s="1">
+      <c r="T24" s="1">
         <v>-1000</v>
       </c>
-      <c r="T24" s="1">
+      <c r="U24" s="1">
         <v>-100</v>
       </c>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1">
+      <c r="V24" s="1"/>
+      <c r="W24" s="1">
         <v>-750</v>
       </c>
-      <c r="W24" s="2">
+      <c r="X24" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>122100</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2024</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D25" s="1">
         <f t="shared" si="1"/>
         <v>122100</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>50000</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-500</v>
       </c>
-      <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1">
+      <c r="H25" s="1"/>
+      <c r="I25" s="1">
         <v>-4500</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>-200</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <v>-20000</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>-10000</v>
       </c>
-      <c r="L25" s="1">
+      <c r="M25" s="1">
         <v>-400</v>
       </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1">
         <v>-500</v>
       </c>
-      <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="1">
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1">
         <v>-30000</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="R25" s="1">
         <v>0</v>
       </c>
-      <c r="R25" s="1">
+      <c r="S25" s="1">
         <v>-500</v>
       </c>
-      <c r="S25" s="1">
+      <c r="T25" s="1">
         <v>-1000</v>
       </c>
-      <c r="T25" s="1">
+      <c r="U25" s="1">
         <v>-100</v>
       </c>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1">
+      <c r="V25" s="1"/>
+      <c r="W25" s="1">
         <v>-750</v>
       </c>
-      <c r="W25" s="2">
+      <c r="X25" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>103650</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2024</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D26" s="1">
         <f t="shared" si="1"/>
         <v>103650</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>33000</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1">
+      <c r="H26" s="1"/>
+      <c r="I26" s="1">
         <v>-4500</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <v>-200</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1">
+      <c r="K26" s="1"/>
+      <c r="L26" s="1">
         <v>-10000</v>
       </c>
-      <c r="L26" s="1">
+      <c r="M26" s="1">
         <v>-400</v>
       </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1">
         <v>-500</v>
       </c>
-      <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="1">
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1">
         <v>0</v>
       </c>
-      <c r="R26" s="1">
+      <c r="S26" s="1">
         <v>-500</v>
       </c>
-      <c r="S26" s="1">
+      <c r="T26" s="1">
         <v>-1000</v>
       </c>
-      <c r="T26" s="1">
+      <c r="U26" s="1">
         <v>-100</v>
       </c>
-      <c r="U26" s="1">
+      <c r="V26" s="1">
         <v>-1000</v>
       </c>
-      <c r="V26" s="1">
+      <c r="W26" s="1">
         <v>-750</v>
       </c>
-      <c r="W26" s="2">
+      <c r="X26" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>117700</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2024</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D27" s="1">
         <f t="shared" si="1"/>
         <v>117700</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>40000</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-400</v>
       </c>
-      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1">
+      <c r="H27" s="1"/>
+      <c r="I27" s="1">
         <v>-4500</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>-200</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <v>-20000</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>-10000</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <v>-400</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <v>-500</v>
       </c>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1">
+      <c r="O27" s="1"/>
+      <c r="P27" s="1">
         <f t="shared" si="0"/>
         <v>-4500</v>
       </c>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1">
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1">
         <v>0</v>
       </c>
-      <c r="R27" s="1">
+      <c r="S27" s="1">
         <v>-500</v>
       </c>
-      <c r="S27" s="1">
+      <c r="T27" s="1">
         <v>-1000</v>
       </c>
-      <c r="T27" s="1">
+      <c r="U27" s="1">
         <v>-100</v>
       </c>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1">
+      <c r="V27" s="1"/>
+      <c r="W27" s="1">
         <v>-750</v>
       </c>
-      <c r="W27" s="2">
+      <c r="X27" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>114850</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2024</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D28" s="1">
         <f t="shared" si="1"/>
         <v>114850</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>40000</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-400</v>
       </c>
-      <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1">
+      <c r="H28" s="1"/>
+      <c r="I28" s="1">
         <v>-4500</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>-200</v>
       </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1">
+      <c r="K28" s="1"/>
+      <c r="L28" s="1">
         <v>-10000</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="1">
         <v>-400</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1">
         <v>-500</v>
       </c>
-      <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="1">
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1">
         <v>0</v>
       </c>
-      <c r="R28" s="1">
+      <c r="S28" s="1">
         <v>-500</v>
       </c>
-      <c r="S28" s="1">
+      <c r="T28" s="1">
         <v>-1000</v>
       </c>
-      <c r="T28" s="1">
+      <c r="U28" s="1">
         <v>-100</v>
       </c>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1">
+      <c r="V28" s="1"/>
+      <c r="W28" s="1">
         <v>-750</v>
       </c>
-      <c r="W28" s="2">
+      <c r="X28" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>136500</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2024</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D29" s="1">
         <f t="shared" si="1"/>
         <v>136500</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>40000</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-400</v>
       </c>
-      <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1">
         <v>-4500</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <v>-200</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <v>-20000</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>-10000</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <v>-400</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <v>-500</v>
       </c>
-      <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="1">
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1">
         <v>0</v>
       </c>
-      <c r="R29" s="1">
+      <c r="S29" s="1">
         <v>-500</v>
       </c>
-      <c r="S29" s="1">
+      <c r="T29" s="1">
         <v>-1000</v>
       </c>
-      <c r="T29" s="1">
+      <c r="U29" s="1">
         <v>-100</v>
       </c>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1">
+      <c r="V29" s="1"/>
+      <c r="W29" s="1">
         <v>-750</v>
       </c>
-      <c r="W29" s="2">
+      <c r="X29" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>138150</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2024</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" s="1">
         <f t="shared" si="1"/>
         <v>138150</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>40000</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-400</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1">
         <v>-8000</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>-4500</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <v>-200</v>
       </c>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1">
+      <c r="K30" s="1"/>
+      <c r="L30" s="1">
         <v>-10000</v>
       </c>
-      <c r="L30" s="1">
+      <c r="M30" s="1">
         <v>-400</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1">
         <v>-500</v>
       </c>
-      <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-      <c r="Q30" s="1">
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1">
         <v>0</v>
       </c>
-      <c r="R30" s="1">
+      <c r="S30" s="1">
         <v>-500</v>
       </c>
-      <c r="S30" s="1">
+      <c r="T30" s="1">
         <v>-1000</v>
       </c>
-      <c r="T30" s="1">
+      <c r="U30" s="1">
         <v>-100</v>
       </c>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1">
+      <c r="V30" s="1"/>
+      <c r="W30" s="1">
         <v>-750</v>
       </c>
-      <c r="W30" s="2">
+      <c r="X30" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>151800</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2024</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D31" s="1">
         <f t="shared" si="1"/>
         <v>151800</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>40000</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-400</v>
       </c>
-      <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1">
         <v>-4500</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>-200</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <v>-60000</v>
       </c>
-      <c r="K31" s="1">
+      <c r="L31" s="1">
         <v>-10000</v>
       </c>
-      <c r="L31" s="1">
+      <c r="M31" s="1">
         <v>-400</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <v>-500</v>
       </c>
-      <c r="N31" s="1">
+      <c r="O31" s="1">
         <v>-1200</v>
       </c>
-      <c r="O31" s="1">
+      <c r="P31" s="1">
         <f t="shared" si="0"/>
         <v>-4500</v>
       </c>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1">
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1">
         <v>0</v>
       </c>
-      <c r="R31" s="1">
+      <c r="S31" s="1">
         <v>-500</v>
       </c>
-      <c r="S31" s="1">
+      <c r="T31" s="1">
         <v>-1000</v>
       </c>
-      <c r="T31" s="1">
+      <c r="U31" s="1">
         <v>-100</v>
       </c>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1">
+      <c r="V31" s="1"/>
+      <c r="W31" s="1">
         <v>-750</v>
       </c>
-      <c r="W31" s="2">
+      <c r="X31" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>107750</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2024</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D32" s="1">
         <f t="shared" si="1"/>
         <v>107750</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>50000</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-500</v>
       </c>
-      <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1">
         <v>-4500</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>-200</v>
       </c>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1">
+      <c r="K32" s="1"/>
+      <c r="L32" s="1">
         <v>-10000</v>
       </c>
-      <c r="L32" s="1">
+      <c r="M32" s="1">
         <v>-400</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1">
         <v>-500</v>
       </c>
-      <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1">
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1">
         <v>-40000</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="R32" s="1">
         <v>0</v>
       </c>
-      <c r="R32" s="1">
+      <c r="S32" s="1">
         <v>-500</v>
       </c>
-      <c r="S32" s="1">
+      <c r="T32" s="1">
         <v>-1000</v>
       </c>
-      <c r="T32" s="1">
+      <c r="U32" s="1">
         <v>-100</v>
       </c>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1">
+      <c r="V32" s="1"/>
+      <c r="W32" s="1">
         <v>-750</v>
       </c>
-      <c r="W32" s="2">
+      <c r="X32" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>99300</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2024</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D33" s="1">
         <f t="shared" si="1"/>
         <v>99300</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>82000</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-820</v>
       </c>
-      <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1">
         <v>-4500</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>-200</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <v>-20000</v>
       </c>
-      <c r="K33" s="1">
+      <c r="L33" s="1">
         <v>-10000</v>
       </c>
-      <c r="L33" s="1">
+      <c r="M33" s="1">
         <v>-400</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <v>-500</v>
       </c>
-      <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
-      <c r="Q33" s="1">
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1">
         <v>0</v>
       </c>
-      <c r="R33" s="1">
+      <c r="S33" s="1">
         <v>-500</v>
       </c>
-      <c r="S33" s="1">
+      <c r="T33" s="1">
         <v>-1000</v>
       </c>
-      <c r="T33" s="1">
+      <c r="U33" s="1">
         <v>-100</v>
       </c>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1">
+      <c r="V33" s="1"/>
+      <c r="W33" s="1">
         <v>-750</v>
       </c>
-      <c r="W33" s="2">
+      <c r="X33" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>142530</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2024</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D34" s="1">
         <f t="shared" si="1"/>
         <v>142530</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>45000</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-450</v>
       </c>
-      <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1">
         <v>-4500</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34" s="1">
         <v>-200</v>
       </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1">
+      <c r="K34" s="1"/>
+      <c r="L34" s="1">
         <v>-10000</v>
       </c>
-      <c r="L34" s="1">
+      <c r="M34" s="1">
         <v>-400</v>
       </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1">
         <v>-500</v>
       </c>
-      <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
-      <c r="Q34" s="1">
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1">
         <v>0</v>
       </c>
-      <c r="R34" s="1">
+      <c r="S34" s="1">
         <v>-500</v>
       </c>
-      <c r="S34" s="1">
+      <c r="T34" s="1">
         <v>-1000</v>
       </c>
-      <c r="T34" s="1">
+      <c r="U34" s="1">
         <v>-100</v>
       </c>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1">
+      <c r="V34" s="1"/>
+      <c r="W34" s="1">
         <v>-750</v>
       </c>
-      <c r="W34" s="2">
+      <c r="X34" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>169130</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2024</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D35" s="1">
         <f t="shared" si="1"/>
         <v>169130</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>45000</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-450</v>
       </c>
-      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1">
+      <c r="H35" s="1"/>
+      <c r="I35" s="1">
         <v>-4500</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <v>-200</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <v>-20000</v>
       </c>
-      <c r="K35" s="1">
+      <c r="L35" s="1">
         <v>-10000</v>
       </c>
-      <c r="L35" s="1">
+      <c r="M35" s="1">
         <v>-400</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <v>-500</v>
       </c>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1">
+      <c r="O35" s="1"/>
+      <c r="P35" s="1">
         <f t="shared" si="0"/>
         <v>-4500</v>
       </c>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1">
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1">
         <v>0</v>
       </c>
-      <c r="R35" s="1">
+      <c r="S35" s="1">
         <v>-500</v>
       </c>
-      <c r="S35" s="1">
+      <c r="T35" s="1">
         <v>-1000</v>
       </c>
-      <c r="T35" s="1">
+      <c r="U35" s="1">
         <v>-100</v>
       </c>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1">
+      <c r="V35" s="1"/>
+      <c r="W35" s="1">
         <v>-750</v>
       </c>
-      <c r="W35" s="2">
+      <c r="X35" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>171230</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2025</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D36" s="1">
         <f t="shared" si="1"/>
         <v>171230</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>45000</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-450</v>
       </c>
-      <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1">
         <v>-4500</v>
       </c>
-      <c r="I36" s="1">
+      <c r="J36" s="1">
         <v>-200</v>
       </c>
-      <c r="J36" s="1">
+      <c r="K36" s="1">
         <v>-20000</v>
       </c>
-      <c r="K36" s="1">
+      <c r="L36" s="1">
         <v>-10000</v>
       </c>
-      <c r="L36" s="1">
+      <c r="M36" s="1">
         <v>-400</v>
       </c>
-      <c r="M36" s="1">
+      <c r="N36" s="1">
         <v>-500</v>
       </c>
-      <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
-      <c r="R36" s="1">
+      <c r="R36" s="1"/>
+      <c r="S36" s="1">
         <v>-500</v>
       </c>
-      <c r="S36" s="1">
+      <c r="T36" s="1">
         <v>-1000</v>
       </c>
-      <c r="T36" s="1">
+      <c r="U36" s="1">
         <v>-100</v>
       </c>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1">
+      <c r="V36" s="1"/>
+      <c r="W36" s="1">
         <v>-750</v>
       </c>
-      <c r="W36" s="2">
+      <c r="X36" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>177830</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2025</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D37" s="1">
         <f t="shared" si="1"/>
         <v>177830</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>45000</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <f>IF(Budget_Table[[#This Row],[Revenue]]&gt;39999,Budget_Table[[#This Row],[Revenue]]*-0.01,0)</f>
         <v>-450</v>
       </c>
-      <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1">
+      <c r="H37" s="1"/>
+      <c r="I37" s="1">
         <v>-4500</v>
       </c>
-      <c r="I37" s="1">
+      <c r="J37" s="1">
         <v>-200</v>
       </c>
-      <c r="J37" s="1">
+      <c r="K37" s="1">
         <v>-20000</v>
       </c>
-      <c r="K37" s="1">
+      <c r="L37" s="1">
         <v>-10000</v>
       </c>
-      <c r="L37" s="1">
+      <c r="M37" s="1">
         <v>-400</v>
       </c>
-      <c r="M37" s="1">
+      <c r="N37" s="1">
         <v>-500</v>
       </c>
-      <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="1">
+      <c r="R37" s="1"/>
+      <c r="S37" s="1">
         <v>-500</v>
       </c>
-      <c r="S37" s="1">
+      <c r="T37" s="1">
         <v>-1000</v>
       </c>
-      <c r="T37" s="1">
+      <c r="U37" s="1">
         <v>-100</v>
       </c>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1">
+      <c r="V37" s="1"/>
+      <c r="W37" s="1">
         <v>-750</v>
       </c>
-      <c r="W37" s="2">
+      <c r="X37" s="2">
         <f>SUM(Budget_Table[[#This Row],[Bank_Balance]:[Fuel]])</f>
         <v>184430</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
         <f>SUBTOTAL(103,Budget_Table[Month])</f>
         <v>36</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1">
         <f>SUBTOTAL(104,Budget_Table[Bank_Balance])</f>
         <v>177830</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <f>SUBTOTAL(101,Budget_Table[Revenue])</f>
         <v>44055.555555555555</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <f>SUBTOTAL(101,Budget_Table[Bonus])</f>
         <v>-313.05555555555554</v>
       </c>
-      <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1">
+      <c r="H38" s="1"/>
+      <c r="I38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Salaries])</f>
         <v>-152000</v>
       </c>
-      <c r="I38" s="1">
+      <c r="J38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Maint])</f>
         <v>-7200</v>
       </c>
-      <c r="J38" s="1">
+      <c r="K38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Stock])</f>
         <v>-530000</v>
       </c>
-      <c r="K38" s="1">
+      <c r="L38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Home_Expenses])</f>
         <v>-363500</v>
       </c>
-      <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
-      <c r="O38" s="1">
+      <c r="O38" s="1"/>
+      <c r="P38" s="1">
         <f>SUBTOTAL(101,Budget_Table[Cloths])</f>
         <v>-4500</v>
       </c>
-      <c r="P38" s="1">
+      <c r="Q38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Schools])</f>
         <v>-188000</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="R38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Education])</f>
         <v>-36000</v>
       </c>
-      <c r="R38" s="1">
+      <c r="S38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Internet])</f>
         <v>-17750</v>
       </c>
-      <c r="S38" s="1">
+      <c r="T38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Electric])</f>
         <v>-35400</v>
       </c>
-      <c r="T38" s="1">
+      <c r="U38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Gas])</f>
         <v>-3600</v>
       </c>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1">
+      <c r="V38" s="1"/>
+      <c r="W38" s="1">
         <f>SUBTOTAL(109,Budget_Table[Fuel])</f>
         <v>-26850</v>
       </c>
-      <c r="W38" s="1">
+      <c r="X38" s="1">
         <f>SUBTOTAL(104,Budget_Table[Balance])</f>
         <v>184430</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>240</v>
       </c>
       <c r="B44">
-        <f t="array" ref="B44:B46">_xlfn.MODE.MULT(D2:D37)</f>
+        <f t="array" ref="B44:B46">_xlfn.MODE.MULT(E2:E37)</f>
         <v>40000</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>45000</v>
       </c>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B46" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>255</v>
       </c>
@@ -16869,17 +17016,17 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E38 H2:V38 F2:G5 F6 F7:G22">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="lessThan">
+  <conditionalFormatting sqref="F2:F38 I2:W38 G2:H5 G6 G7:H22">
+    <cfRule type="cellIs" dxfId="31" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W37">
-    <cfRule type="top10" dxfId="5" priority="12" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="4" priority="13" percent="1" rank="10"/>
+  <conditionalFormatting sqref="X2:X37">
+    <cfRule type="top10" dxfId="30" priority="12" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C38">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="D2:D38">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18238,7 +18385,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E37 C69:D69">
-    <cfRule type="cellIs" dxfId="2" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="greaterThan">
       <formula>$C$67*0.03</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18428,7 +18575,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -20357,7 +20504,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D28:D31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20490,7 +20637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D630934-E6BF-4D61-ABF9-FF9E611BB503}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
@@ -20660,11 +20807,11 @@
     </row>
     <row r="2" spans="1:2" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="str">
-        <f xml:space="preserve"> CONCATENATE("Our Initial Bank Budget Balance Was ",TEXT('01-Budget'!C2,"0.0"))</f>
+        <f xml:space="preserve"> CONCATENATE("Our Initial Bank Budget Balance Was ",TEXT('01-Budget'!D2,"0.0"))</f>
         <v>Our Initial Bank Budget Balance Was 70000.0</v>
       </c>
       <c r="B2" s="12">
-        <f>'01-Budget'!C2</f>
+        <f>'01-Budget'!D2</f>
         <v>70000</v>
       </c>
     </row>

</xml_diff>